<commit_message>
Move facts to separate files on spark side
</commit_message>
<xml_diff>
--- a/src/Backend/pie.xlsx
+++ b/src/Backend/pie.xlsx
@@ -142,10 +142,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,7 +528,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>